<commit_message>
add data tables/sources and on the graphics
</commit_message>
<xml_diff>
--- a/data_sources.xlsx
+++ b/data_sources.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Thesis_Model_report/newsources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Presentation_thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1680A33-3631-1942-9BA8-A9BC772214FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478AB244-D0E9-3A4F-A17D-57233A3A90FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{F1DC5997-B81C-1D4C-A161-165DD2CF14C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{F1DC5997-B81C-1D4C-A161-165DD2CF14C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="explication.tx.change" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>tx.change</t>
   </si>
@@ -59,9 +60,6 @@
     <t>Variable</t>
   </si>
   <si>
-    <t>1960 - 2022</t>
-  </si>
-  <si>
     <t>HTG/USD</t>
   </si>
   <si>
@@ -99,6 +97,12 @@
   </si>
   <si>
     <t>exp</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>une moyenne annuelle sur la base des moyennes mensuelles.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD8EBDE-6A7C-074F-9398-504B627F2B93}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -526,16 +530,16 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>4</v>
@@ -544,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1570,99 +1574,144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A51A81E5-33FB-5D4F-84DA-90DBB0281FD0}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="225.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="225.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E10382-C4D9-8A41-8487-DFC2AF9819A3}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="225.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>